<commit_message>
implemente una base de datos por si en un futuro se quieren hacer peticiones d e los reportes
</commit_message>
<xml_diff>
--- a/reporte_final.xlsx
+++ b/reporte_final.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -440,42 +436,44 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Proveedor</t>
+          <t>proveedor</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Producto</t>
+          <t>producto</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Cantidad</t>
+          <t>cantidad</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>PrecioUnitario</t>
+          <t>precio_unitario</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>PrecioTotal</t>
+          <t>precio_total</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45787</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">LogiMax </t>
+          <t>LogiMax</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -494,12 +492,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45789</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">LogiMax </t>
+          <t>LogiMax</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -518,12 +518,14 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45791</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LogiMax </t>
+          <t>LogiMax</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -542,12 +544,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45794</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">LogiMax </t>
+          <t>LogiMax</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -566,8 +570,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45789</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -590,8 +596,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45791</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -614,8 +622,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>45792</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -638,8 +648,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45795</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -662,12 +674,14 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45791</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">NovaIndustrias </t>
+          <t>NovaIndustrias</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -688,12 +702,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16/05/2025</t>
+          <t>2025-05-16</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">NovaIndustrias </t>
+          <t>NovaIndustrias</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -712,12 +726,14 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>45794</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">NovaIndustrias </t>
+          <t>NovaIndustrias</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -736,12 +752,14 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>45797</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">NovaIndustrias </t>
+          <t>NovaIndustrias</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -760,8 +778,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>45790</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -784,8 +804,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>45792</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -808,8 +830,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>45794</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -832,8 +856,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>45795</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>

</xml_diff>